<commit_message>
Changes to be committed: 	modified:   Broker_Analysis.xlsx
</commit_message>
<xml_diff>
--- a/Broker_Analysis.xlsx
+++ b/Broker_Analysis.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayush\OneDrive\Desktop\Others\python scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CABF673-423C-4B1E-A759-51CC0972FEA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C9F1B4-56F4-4B4C-B82E-3F48E52867E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2025_06_09" sheetId="11" r:id="rId1"/>
+    <sheet name="2025_06_10" sheetId="11" r:id="rId1"/>
     <sheet name="2025-06-09" sheetId="10" r:id="rId2"/>
     <sheet name="2025-06-08" sheetId="9" r:id="rId3"/>
     <sheet name="2025-06-05" sheetId="8" r:id="rId4"/>
@@ -14967,7 +14967,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FEE11C3-3B44-4022-BB32-BDF73F267C1B}">
   <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
🔄 Update Broker_Analysis.xlsx from Repo A
</commit_message>
<xml_diff>
--- a/Broker_Analysis.xlsx
+++ b/Broker_Analysis.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="2025-06-17" sheetId="1" r:id="rId1"/>
+    <sheet name="2025-06-18" sheetId="1" r:id="rId1"/>
     <sheet name="2025-06-16" sheetId="2" r:id="rId2"/>
     <sheet name="2025-06-15" sheetId="3" r:id="rId3"/>
     <sheet name="2025-06-12" sheetId="4" r:id="rId4"/>
@@ -442,19 +442,19 @@
         <v>B1</v>
       </c>
       <c r="B2" t="str">
-        <v>CHDC/12651/2,605.46</v>
+        <v>NRN/17001/2,027.74</v>
       </c>
       <c r="C2" t="str">
-        <v>RADHI/37986/807.48</v>
+        <v>CHDC/12676/2,605.40</v>
       </c>
       <c r="D2" t="str">
-        <v>NRN/15193/2,030.46</v>
+        <v>RADHI/38877/809.05</v>
       </c>
       <c r="E2" t="str">
-        <v>NIFRA/94673/283.11</v>
+        <v>NIFRA/95882/283.06</v>
       </c>
       <c r="F2" t="str">
-        <v>SHIVM/50743/521.51</v>
+        <v>SHIVM/46246/521.29</v>
       </c>
     </row>
     <row r="3">
@@ -462,19 +462,19 @@
         <v>B3</v>
       </c>
       <c r="B3" t="str">
-        <v>SHIVM/20067/527.69</v>
+        <v>OMPL/7080/1,565.30</v>
       </c>
       <c r="C3" t="str">
-        <v>OMPL/6830/1,568.73</v>
+        <v>SHIVM/19743/526.52</v>
       </c>
       <c r="D3" t="str">
         <v>HLI/19806/405.08</v>
       </c>
       <c r="E3" t="str">
-        <v>MBL/34448/220.88</v>
+        <v>MBL/35858/220.82</v>
       </c>
       <c r="F3" t="str">
-        <v>HIDCLP/26056/217.20</v>
+        <v>HIDCLP/25556/217.19</v>
       </c>
     </row>
     <row r="4">
@@ -482,19 +482,19 @@
         <v>B4</v>
       </c>
       <c r="B4" t="str">
-        <v>SARBTM/88309/844.08</v>
+        <v>SARBTM/87176/844.05</v>
       </c>
       <c r="C4" t="str">
-        <v>HRL/40905/933.53</v>
+        <v>GMFIL/78775/490.03</v>
       </c>
       <c r="D4" t="str">
-        <v>GMFIL/57843/490.92</v>
+        <v>UMRH/44636/610.11</v>
       </c>
       <c r="E4" t="str">
-        <v>UMRH/44436/610.21</v>
+        <v>HRL/20951/932.75</v>
       </c>
       <c r="F4" t="str">
-        <v>FMDBL/25833/750.10</v>
+        <v>FMDBL/26224/750.27</v>
       </c>
     </row>
     <row r="5">
@@ -502,19 +502,19 @@
         <v>B5</v>
       </c>
       <c r="B5" t="str">
-        <v>HIDCLP/106453/211.79</v>
+        <v>HIDCLP/110522/212.11</v>
       </c>
       <c r="C5" t="str">
-        <v>CHDC/4906/2,610.10</v>
+        <v>CHDC/6013/2,604.81</v>
       </c>
       <c r="D5" t="str">
-        <v>HRL/11763/954.73</v>
+        <v>HRL/11764/954.30</v>
       </c>
       <c r="E5" t="str">
-        <v>NGPL/21315/392.76</v>
+        <v>NGPL/19361/392.99</v>
       </c>
       <c r="F5" t="str">
-        <v>LBBL/16027/446.39</v>
+        <v>RADHI/9254/794.46</v>
       </c>
     </row>
     <row r="6">
@@ -522,19 +522,19 @@
         <v>B6</v>
       </c>
       <c r="B6" t="str">
-        <v>NRIC/511017/1,296.17</v>
+        <v>NRIC/509644/1,296.10</v>
       </c>
       <c r="C6" t="str">
-        <v>UPCL/164472/447.41</v>
+        <v>UPCL/161522/447.47</v>
       </c>
       <c r="D6" t="str">
-        <v>RIDI/182082/278.36</v>
+        <v>RIDI/171430/278.43</v>
       </c>
       <c r="E6" t="str">
-        <v>HRL/49553/946.63</v>
+        <v>HRL/48336/944.91</v>
       </c>
       <c r="F6" t="str">
-        <v>SHPC/56628/606.37</v>
+        <v>SHPC/70172/610.00</v>
       </c>
     </row>
     <row r="7">
@@ -542,19 +542,19 @@
         <v>B7</v>
       </c>
       <c r="B7" t="str">
-        <v>NRN/16190/2,047.66</v>
+        <v>NRN/16146/2,047.66</v>
       </c>
       <c r="C7" t="str">
-        <v>CHDC/10617/2,591.01</v>
+        <v>CHDC/10758/2,590.68</v>
       </c>
       <c r="D7" t="str">
-        <v>RADHI/30625/793.62</v>
+        <v>RADHI/29453/793.82</v>
       </c>
       <c r="E7" t="str">
-        <v>GHL/44550/257.68</v>
+        <v>SHPC/26755/622.22</v>
       </c>
       <c r="F7" t="str">
-        <v>SIFC/17925/575.31</v>
+        <v>GHL/60743/257.76</v>
       </c>
     </row>
     <row r="8">
@@ -562,19 +562,19 @@
         <v>B8</v>
       </c>
       <c r="B8" t="str">
-        <v>NGPL/239238/406.30</v>
+        <v>NGPL/320160/406.99</v>
       </c>
       <c r="C8" t="str">
-        <v>SADBL/68270/426.71</v>
+        <v>SADBL/67564/426.61</v>
       </c>
       <c r="D8" t="str">
-        <v>HIDCLP/138553/214.09</v>
+        <v>LSL/107189/223.82</v>
       </c>
       <c r="E8" t="str">
-        <v>LSL/107199/223.82</v>
+        <v>SAHAS/28257/557.30</v>
       </c>
       <c r="F8" t="str">
-        <v>SAHAS/38589/557.31</v>
+        <v>HIDCLP/76756/214.12</v>
       </c>
     </row>
     <row r="9">
@@ -582,19 +582,19 @@
         <v>B10</v>
       </c>
       <c r="B9" t="str">
-        <v>HIDCLP/74910/213.64</v>
+        <v>HIDCLP/73210/213.65</v>
       </c>
       <c r="C9" t="str">
-        <v>SHPC/16847/628.80</v>
+        <v>SHPC/21967/639.26</v>
       </c>
       <c r="D9" t="str">
-        <v>CIT/3631/1,920.87</v>
+        <v>CIT/3688/1,920.53</v>
       </c>
       <c r="E9" t="str">
-        <v>NTC/7525/871.57</v>
+        <v>NTC/7545/871.51</v>
       </c>
       <c r="F9" t="str">
-        <v>CHCL/9748/576.51</v>
+        <v>CHCL/10280/576.52</v>
       </c>
     </row>
     <row r="10">
@@ -602,19 +602,19 @@
         <v>B11</v>
       </c>
       <c r="B10" t="str">
-        <v>NABIL/16539/497.00</v>
+        <v>NABIL/16144/497.00</v>
       </c>
       <c r="C10" t="str">
-        <v>CIT/3616/1,907.86</v>
+        <v>CIT/3631/1,907.81</v>
       </c>
       <c r="D10" t="str">
-        <v>RHPL/15456/413.63</v>
+        <v>RHPL/15276/413.64</v>
       </c>
       <c r="E10" t="str">
         <v>ALICL/8006/657.38</v>
       </c>
       <c r="F10" t="str">
-        <v>SINDU/6536/842.01</v>
+        <v>SONA/10096/459.35</v>
       </c>
     </row>
     <row r="11">
@@ -622,19 +622,19 @@
         <v>B13</v>
       </c>
       <c r="B11" t="str">
-        <v>UMHL/26133/520.49</v>
+        <v>UMHL/34961/523.89</v>
       </c>
       <c r="C11" t="str">
-        <v>NGPL/31759/392.88</v>
+        <v>NGPL/31179/393.57</v>
       </c>
       <c r="D11" t="str">
-        <v>CORBL/3953/2,541.59</v>
+        <v>HRL/10404/968.30</v>
       </c>
       <c r="E11" t="str">
-        <v>HRL/8232/972.72</v>
+        <v>CORBL/3903/2,541.59</v>
       </c>
       <c r="F11" t="str">
-        <v>CREST/3208/1,895.82</v>
+        <v>SHPC/12386/620.31</v>
       </c>
     </row>
     <row r="12">
@@ -642,19 +642,19 @@
         <v>B14</v>
       </c>
       <c r="B12" t="str">
-        <v>CGH/78690/950.06</v>
+        <v>CGH/65250/955.42</v>
       </c>
       <c r="C12" t="str">
-        <v>HRL/34999/941.25</v>
+        <v>HRL/34995/940.73</v>
       </c>
       <c r="D12" t="str">
-        <v>CHCL/49038/576.70</v>
+        <v>BARUN/67146/384.99</v>
       </c>
       <c r="E12" t="str">
-        <v>HIDCLP/137258/211.44</v>
+        <v>CHCL/42142/576.66</v>
       </c>
       <c r="F12" t="str">
-        <v>BARUN/59339/385.73</v>
+        <v>SAHAS/48843/538.70</v>
       </c>
     </row>
     <row r="13">
@@ -662,19 +662,19 @@
         <v>B16</v>
       </c>
       <c r="B13" t="str">
-        <v>RADHI/125150/817.92</v>
+        <v>RADHI/114828/818.05</v>
       </c>
       <c r="C13" t="str">
-        <v>CHDC/32796/2,689.43</v>
+        <v>CHDC/34305/2,680.31</v>
       </c>
       <c r="D13" t="str">
-        <v>SHL/66506/570.41</v>
+        <v>SHL/69604/570.97</v>
       </c>
       <c r="E13" t="str">
-        <v>NMIC/17206/1,835.09</v>
+        <v>NMIC/17161/1,834.74</v>
       </c>
       <c r="F13" t="str">
-        <v>CREST/17108/1,802.74</v>
+        <v>CREST/17118/1,801.00</v>
       </c>
     </row>
     <row r="14">
@@ -682,19 +682,19 @@
         <v>B17</v>
       </c>
       <c r="B14" t="str">
-        <v>NGPL/421159/401.04</v>
+        <v>NGPL/468845/401.68</v>
       </c>
       <c r="C14" t="str">
-        <v>HIDCLP/710498/215.97</v>
+        <v>HIDCLP/710188/216.03</v>
       </c>
       <c r="D14" t="str">
-        <v>HIDCL/204027/312.46</v>
+        <v>HIDCL/208968/312.21</v>
       </c>
       <c r="E14" t="str">
-        <v>MEN/91906/616.54</v>
+        <v>MEN/97946/617.29</v>
       </c>
       <c r="F14" t="str">
-        <v>SADBL/73062/426.43</v>
+        <v>SADBL/73122/426.41</v>
       </c>
     </row>
     <row r="15">
@@ -705,16 +705,16 @@
         <v>SPIL/23534/814.90</v>
       </c>
       <c r="C15" t="str">
-        <v>RADHI/16965/801.86</v>
+        <v>RADHI/15264/802.45</v>
       </c>
       <c r="D15" t="str">
-        <v>NLICL/19263/611.26</v>
+        <v>NLICL/19110/611.26</v>
       </c>
       <c r="E15" t="str">
-        <v>NLIC/12705/752.94</v>
+        <v>NRN/5527/2,032.72</v>
       </c>
       <c r="F15" t="str">
-        <v>NRN/4527/2,040.05</v>
+        <v>NLIC/12711/752.90</v>
       </c>
     </row>
     <row r="16">
@@ -722,19 +722,19 @@
         <v>B19</v>
       </c>
       <c r="B16" t="str">
-        <v>BPCL/107649/653.05</v>
+        <v>BPCL/74978/654.94</v>
       </c>
       <c r="C16" t="str">
-        <v>CHDC/9441/2,661.60</v>
+        <v>CHDC/9291/2,661.60</v>
       </c>
       <c r="D16" t="str">
-        <v>LBBL/31857/464.86</v>
+        <v>SPDL/60891/414.75</v>
       </c>
       <c r="E16" t="str">
-        <v>NADEP/15366/850.57</v>
+        <v>LBBL/30857/464.86</v>
       </c>
       <c r="F16" t="str">
-        <v>OMPL/6075/1,760.61</v>
+        <v>SAPDBL/13744/993.74</v>
       </c>
     </row>
     <row r="17">
@@ -742,19 +742,19 @@
         <v>B20</v>
       </c>
       <c r="B17" t="str">
-        <v>CHDC/7616/2,572.49</v>
+        <v>CHDC/7815/2,571.94</v>
       </c>
       <c r="C17" t="str">
+        <v>SHIVM/35099/522.59</v>
+      </c>
+      <c r="D17" t="str">
+        <v>NRN/8565/2,011.80</v>
+      </c>
+      <c r="E17" t="str">
         <v>SHPC/27806/616.32</v>
       </c>
-      <c r="D17" t="str">
-        <v>SHIVM/30099/523.00</v>
-      </c>
-      <c r="E17" t="str">
-        <v>RADHI/19815/798.59</v>
-      </c>
       <c r="F17" t="str">
-        <v>NRIC/12257/1,266.54</v>
+        <v>NRIC/12257/1,266.04</v>
       </c>
     </row>
     <row r="18">
@@ -762,19 +762,19 @@
         <v>B21</v>
       </c>
       <c r="B18" t="str">
-        <v>SHPC/49389/611.71</v>
+        <v>SHPC/56015/614.40</v>
       </c>
       <c r="C18" t="str">
-        <v>SHIVM/58892/521.47</v>
+        <v>SHIVM/66612/520.58</v>
       </c>
       <c r="D18" t="str">
-        <v>HIDCLP/79377/218.04</v>
+        <v>HIDCLP/85843/217.97</v>
       </c>
       <c r="E18" t="str">
-        <v>SMHL/13436/1,059.24</v>
+        <v>SMHL/15526/1,056.27</v>
       </c>
       <c r="F18" t="str">
-        <v>HIDCL/42766/306.65</v>
+        <v>HIDCL/42417/306.59</v>
       </c>
     </row>
     <row r="19">
@@ -782,19 +782,19 @@
         <v>B22</v>
       </c>
       <c r="B19" t="str">
-        <v>UPCL/84086/455.51</v>
+        <v>UPCL/84353/455.48</v>
       </c>
       <c r="C19" t="str">
-        <v>SHIVM/56618/525.49</v>
+        <v>SHIVM/59854/525.01</v>
       </c>
       <c r="D19" t="str">
-        <v>KPCL/40467/553.90</v>
+        <v>GHL/77996/259.77</v>
       </c>
       <c r="E19" t="str">
-        <v>GHL/79129/259.78</v>
+        <v>KPCL/36089/553.90</v>
       </c>
       <c r="F19" t="str">
-        <v>UNHPL/31890/390.15</v>
+        <v>BARUN/19209/451.16</v>
       </c>
     </row>
     <row r="20">
@@ -802,19 +802,19 @@
         <v>B25</v>
       </c>
       <c r="B20" t="str">
-        <v>KBL/197172/214.96</v>
+        <v>SHEL/151144/298.69</v>
       </c>
       <c r="C20" t="str">
-        <v>NGPL/81830/401.50</v>
+        <v>NGPL/100883/402.07</v>
       </c>
       <c r="D20" t="str">
-        <v>HIDCL/66797/307.75</v>
+        <v>KBL/198148/214.92</v>
       </c>
       <c r="E20" t="str">
-        <v>NRN/8996/2,048.96</v>
+        <v>HIDCL/77062/307.45</v>
       </c>
       <c r="F20" t="str">
-        <v>SHPC/25829/621.50</v>
+        <v>NRN/10264/2,044.44</v>
       </c>
     </row>
     <row r="21">
@@ -822,19 +822,19 @@
         <v>B26</v>
       </c>
       <c r="B21" t="str">
-        <v>RADHI/149406/803.35</v>
+        <v>RADHI/146480/803.69</v>
       </c>
       <c r="C21" t="str">
-        <v>LBBL/59777/455.29</v>
+        <v>LBBL/61335/454.92</v>
       </c>
       <c r="D21" t="str">
-        <v>NGPL/60764/392.27</v>
+        <v>SHIVM/38757/522.74</v>
       </c>
       <c r="E21" t="str">
-        <v>GHL/66790/257.80</v>
+        <v>GHL/65256/257.81</v>
       </c>
       <c r="F21" t="str">
-        <v>SHIVM/31737/523.26</v>
+        <v>NLIC/20910/757.07</v>
       </c>
     </row>
     <row r="22">
@@ -842,19 +842,19 @@
         <v>B28</v>
       </c>
       <c r="B22" t="str">
-        <v>SAHAS/106346/535.50</v>
+        <v>SAHAS/122691/536.64</v>
       </c>
       <c r="C22" t="str">
-        <v>NIFRA/122359/286.06</v>
+        <v>BPCL/63409/691.45</v>
       </c>
       <c r="D22" t="str">
+        <v>NIFRA/122395/286.06</v>
+      </c>
+      <c r="E22" t="str">
         <v>MNBBL/85315/361.17</v>
       </c>
-      <c r="E22" t="str">
-        <v>BPCL/41690/671.80</v>
-      </c>
       <c r="F22" t="str">
-        <v>UNHPL/61630/399.76</v>
+        <v>CORBL/9680/2,422.33</v>
       </c>
     </row>
     <row r="23">
@@ -862,19 +862,19 @@
         <v>B29</v>
       </c>
       <c r="B23" t="str">
-        <v>BPCL/119112/701.68</v>
+        <v>BPCL/163371/730.19</v>
       </c>
       <c r="C23" t="str">
-        <v>CHDC/9649/2,574.66</v>
+        <v>GRDBL/19732/1,267.40</v>
       </c>
       <c r="D23" t="str">
-        <v>GRDBL/19732/1,267.53</v>
+        <v>CHDC/6159/2,574.40</v>
       </c>
       <c r="E23" t="str">
-        <v>AHPC/45180/296.58</v>
+        <v>AKPL/52942/275.73</v>
       </c>
       <c r="F23" t="str">
-        <v>SHIVM/24946/523.64</v>
+        <v>SHL/22798/582.64</v>
       </c>
     </row>
     <row r="24">
@@ -882,19 +882,19 @@
         <v>B32</v>
       </c>
       <c r="B24" t="str">
-        <v>CHDC/31657/2,588.19</v>
+        <v>CHDC/33708/2,586.71</v>
       </c>
       <c r="C24" t="str">
-        <v>SHL/95313/581.47</v>
+        <v>CGH/83546/992.22</v>
       </c>
       <c r="D24" t="str">
-        <v>CGH/55375/986.15</v>
+        <v>SHL/79913/581.55</v>
       </c>
       <c r="E24" t="str">
-        <v>NRIC/41461/1,280.04</v>
+        <v>NRIC/34050/1,277.37</v>
       </c>
       <c r="F24" t="str">
-        <v>BARUN/82478/385.46</v>
+        <v>BARUN/73335/385.42</v>
       </c>
     </row>
     <row r="25">
@@ -902,19 +902,19 @@
         <v>B33</v>
       </c>
       <c r="B25" t="str">
-        <v>SBL/594848/297.45</v>
+        <v>SBL/593671/297.45</v>
       </c>
       <c r="C25" t="str">
-        <v>CHCL/143180/569.39</v>
+        <v>UPCL/189321/455.75</v>
       </c>
       <c r="D25" t="str">
-        <v>UPCL/163551/455.99</v>
+        <v>EBL/86300/652.66</v>
       </c>
       <c r="E25" t="str">
-        <v>EBL/86300/652.66</v>
+        <v>CHCL/87473/569.46</v>
       </c>
       <c r="F25" t="str">
-        <v>CBBL/39352/905.26</v>
+        <v>CBBL/36915/905.25</v>
       </c>
     </row>
     <row r="26">
@@ -922,19 +922,19 @@
         <v>B34</v>
       </c>
       <c r="B26" t="str">
-        <v>SHPC/276996/617.57</v>
+        <v>SHPC/277571/618.84</v>
       </c>
       <c r="C26" t="str">
-        <v>RADHI/101537/799.44</v>
+        <v>RADHI/93431/800.22</v>
       </c>
       <c r="D26" t="str">
-        <v>HRL/69934/959.92</v>
+        <v>HRL/74163/957.82</v>
       </c>
       <c r="E26" t="str">
-        <v>SHIVM/91345/523.31</v>
+        <v>SHIVM/96995/522.92</v>
       </c>
       <c r="F26" t="str">
-        <v>API/136799/301.66</v>
+        <v>API/148177/301.51</v>
       </c>
     </row>
     <row r="27">
@@ -942,19 +942,19 @@
         <v>B35</v>
       </c>
       <c r="B27" t="str">
-        <v>GBIME/275543/239.97</v>
+        <v>GBIME/280014/239.88</v>
       </c>
       <c r="C27" t="str">
-        <v>UPCL/148472/446.16</v>
+        <v>UPCL/150839/446.24</v>
       </c>
       <c r="D27" t="str">
-        <v>SBL/114837/299.48</v>
+        <v>SBL/109353/299.48</v>
       </c>
       <c r="E27" t="str">
-        <v>HURJA/102485/263.27</v>
+        <v>HURJA/99402/263.36</v>
       </c>
       <c r="F27" t="str">
-        <v>BARUN/43967/400.81</v>
+        <v>SHIVM/46143/521.80</v>
       </c>
     </row>
     <row r="28">
@@ -962,19 +962,19 @@
         <v>B36</v>
       </c>
       <c r="B28" t="str">
-        <v>SBI/167938/411.44</v>
+        <v>SBI/168131/411.41</v>
       </c>
       <c r="C28" t="str">
-        <v>SPDL/57930/417.83</v>
+        <v>SPDL/66194/420.59</v>
       </c>
       <c r="D28" t="str">
-        <v>SHPC/29605/619.97</v>
+        <v>SHPC/30900/621.50</v>
       </c>
       <c r="E28" t="str">
-        <v>BARUN/35593/394.73</v>
+        <v>BARUN/38633/394.03</v>
       </c>
       <c r="F28" t="str">
-        <v>KBL/60103/214.24</v>
+        <v>CHCL/24692/557.03</v>
       </c>
     </row>
     <row r="29">
@@ -982,19 +982,19 @@
         <v>B37</v>
       </c>
       <c r="B29" t="str">
+        <v>MEN/10374/597.24</v>
+      </c>
+      <c r="C29" t="str">
         <v>SHL/9625/586.54</v>
-      </c>
-      <c r="C29" t="str">
-        <v>MEN/9964/596.58</v>
       </c>
       <c r="D29" t="str">
         <v>NRN/2128/2,068.32</v>
       </c>
       <c r="E29" t="str">
+        <v>SINDU/4755/824.60</v>
+      </c>
+      <c r="F29" t="str">
         <v>BHPL/3885/951.93</v>
-      </c>
-      <c r="F29" t="str">
-        <v>OMPL/1973/1,680.83</v>
       </c>
     </row>
     <row r="30">
@@ -1002,19 +1002,19 @@
         <v>B38</v>
       </c>
       <c r="B30" t="str">
-        <v>BPCL/268558/635.68</v>
+        <v>BPCL/279194/642.43</v>
       </c>
       <c r="C30" t="str">
-        <v>SHIVM/84849/523.03</v>
+        <v>SHIVM/84372/522.68</v>
       </c>
       <c r="D30" t="str">
-        <v>MBJC/97589/330.78</v>
+        <v>MBJC/129488/330.43</v>
       </c>
       <c r="E30" t="str">
-        <v>HPPL/62976/521.05</v>
+        <v>HPPL/59392/522.01</v>
       </c>
       <c r="F30" t="str">
-        <v>BARUN/60224/405.48</v>
+        <v>BARUN/64077/403.67</v>
       </c>
     </row>
     <row r="31">
@@ -1022,19 +1022,19 @@
         <v>B39</v>
       </c>
       <c r="B31" t="str">
-        <v>RADHI/305529/815.28</v>
+        <v>RADHI/312955/816.10</v>
       </c>
       <c r="C31" t="str">
-        <v>NRN/33291/2,055.54</v>
+        <v>NRN/32613/2,055.48</v>
       </c>
       <c r="D31" t="str">
-        <v>HPPL/99648/551.13</v>
+        <v>HPPL/102893/551.67</v>
       </c>
       <c r="E31" t="str">
-        <v>UPCL/128582/440.09</v>
+        <v>UPCL/112988/440.23</v>
       </c>
       <c r="F31" t="str">
-        <v>UMHL/37775/521.61</v>
+        <v>AKPL/71118/278.94</v>
       </c>
     </row>
     <row r="32">
@@ -1042,16 +1042,16 @@
         <v>B40</v>
       </c>
       <c r="B32" t="str">
-        <v>BPCL/74120/623.53</v>
+        <v>BPCL/65447/623.53</v>
       </c>
       <c r="C32" t="str">
-        <v>SANIMA/46498/318.19</v>
+        <v>SANIMA/45688/318.19</v>
       </c>
       <c r="D32" t="str">
-        <v>SHIVM/24528/522.19</v>
+        <v>SHIVM/24148/522.04</v>
       </c>
       <c r="E32" t="str">
-        <v>EBL/15302/645.59</v>
+        <v>CIT/5790/1,898.18</v>
       </c>
       <c r="F32" t="str">
         <v>LSL/40897/216.24</v>
@@ -1062,19 +1062,19 @@
         <v>B41</v>
       </c>
       <c r="B33" t="str">
-        <v>SAPDBL/147244/1,031.89</v>
+        <v>SAPDBL/147607/1,031.78</v>
       </c>
       <c r="C33" t="str">
-        <v>RADHI/60536/808.01</v>
+        <v>RADHI/58889/809.09</v>
       </c>
       <c r="D33" t="str">
-        <v>NMIC/18457/1,859.31</v>
+        <v>NMIC/18552/1,857.48</v>
       </c>
       <c r="E33" t="str">
-        <v>SHIVM/49740/522.57</v>
+        <v>SHIVM/52449/522.12</v>
       </c>
       <c r="F33" t="str">
-        <v>BARUN/37178/386.75</v>
+        <v>BARUN/34641/386.65</v>
       </c>
     </row>
     <row r="34">
@@ -1082,19 +1082,19 @@
         <v>B42</v>
       </c>
       <c r="B34" t="str">
-        <v>GBIME/1041235/240.28</v>
+        <v>GBIME/1048791/240.23</v>
       </c>
       <c r="C34" t="str">
-        <v>MERO/111410/746.03</v>
+        <v>MERO/187974/746.04</v>
       </c>
       <c r="D34" t="str">
-        <v>NRN/40149/2,022.06</v>
+        <v>NRN/38832/2,022.02</v>
       </c>
       <c r="E34" t="str">
-        <v>SHIVM/123670/521.85</v>
+        <v>SHIVM/124082/521.62</v>
       </c>
       <c r="F34" t="str">
-        <v>BARUN/106181/390.00</v>
+        <v>HRL/36957/956.09</v>
       </c>
     </row>
     <row r="35">
@@ -1102,19 +1102,19 @@
         <v>B43</v>
       </c>
       <c r="B35" t="str">
-        <v>SPDL/76497/424.08</v>
+        <v>SPDL/56029/425.22</v>
       </c>
       <c r="C35" t="str">
-        <v>SPIL/25918/824.34</v>
+        <v>SPIL/25941/824.30</v>
       </c>
       <c r="D35" t="str">
         <v>USLB/8379/1,979.59</v>
       </c>
       <c r="E35" t="str">
-        <v>SHIVM/31485/522.72</v>
+        <v>SHIVM/32377/521.48</v>
       </c>
       <c r="F35" t="str">
-        <v>NIL/19018/691.78</v>
+        <v>NIL/18088/691.69</v>
       </c>
     </row>
     <row r="36">
@@ -1122,19 +1122,19 @@
         <v>B44</v>
       </c>
       <c r="B36" t="str">
-        <v>CHCL/226289/568.87</v>
+        <v>CHCL/287005/569.52</v>
       </c>
       <c r="C36" t="str">
-        <v>NIFRA/248256/284.47</v>
+        <v>NIFRA/281847/284.03</v>
       </c>
       <c r="D36" t="str">
-        <v>EBL/102902/651.07</v>
+        <v>EBL/97754/651.06</v>
       </c>
       <c r="E36" t="str">
-        <v>UPCL/124691/451.51</v>
+        <v>UPCL/124409/451.54</v>
       </c>
       <c r="F36" t="str">
-        <v>HRL/41643/958.63</v>
+        <v>HIDCL/150846/306.90</v>
       </c>
     </row>
     <row r="37">
@@ -1142,19 +1142,19 @@
         <v>B45</v>
       </c>
       <c r="B37" t="str">
-        <v>MEN/189326/601.41</v>
+        <v>MEN/214101/601.83</v>
       </c>
       <c r="C37" t="str">
-        <v>GBIME/256661/226.34</v>
+        <v>GBIME/258164/226.36</v>
       </c>
       <c r="D37" t="str">
-        <v>SHL/94592/574.26</v>
+        <v>SHL/92683/574.35</v>
       </c>
       <c r="E37" t="str">
-        <v>CZBIL/191207/216.09</v>
+        <v>CZBIL/190222/216.07</v>
       </c>
       <c r="F37" t="str">
-        <v>NRN/16793/2,046.07</v>
+        <v>NRN/17481/2,044.36</v>
       </c>
     </row>
     <row r="38">
@@ -1162,19 +1162,19 @@
         <v>B46</v>
       </c>
       <c r="B38" t="str">
-        <v>HRL/19877/938.93</v>
+        <v>HRL/20125/937.66</v>
       </c>
       <c r="C38" t="str">
-        <v>SHPC/28828/617.10</v>
+        <v>SHPC/29908/617.71</v>
       </c>
       <c r="D38" t="str">
-        <v>SARBTM/13612/840.42</v>
+        <v>AHPC/37001/303.14</v>
       </c>
       <c r="E38" t="str">
-        <v>AHPC/34472/303.42</v>
+        <v>SARBTM/10612/840.42</v>
       </c>
       <c r="F38" t="str">
-        <v>MEN/13946/609.39</v>
+        <v>MEN/14205/609.66</v>
       </c>
     </row>
     <row r="39">
@@ -1182,19 +1182,19 @@
         <v>B47</v>
       </c>
       <c r="B39" t="str">
-        <v>AKPL/154204/274.95</v>
+        <v>AKPL/139474/274.98</v>
       </c>
       <c r="C39" t="str">
-        <v>NGPL/92837/398.31</v>
+        <v>NGPL/88902/398.36</v>
       </c>
       <c r="D39" t="str">
         <v>NRN/7303/2,036.68</v>
       </c>
       <c r="E39" t="str">
-        <v>CREST/8076/1,718.16</v>
+        <v>CREST/8679/1,707.40</v>
       </c>
       <c r="F39" t="str">
-        <v>CHDC/4606/2,630.79</v>
+        <v>CHDC/4376/2,629.40</v>
       </c>
     </row>
     <row r="40">
@@ -1202,19 +1202,19 @@
         <v>B48</v>
       </c>
       <c r="B40" t="str">
-        <v>GHL/359613/264.03</v>
+        <v>GHL/387426/263.80</v>
       </c>
       <c r="C40" t="str">
-        <v>MEN/72998/625.97</v>
+        <v>SHPC/98287/616.47</v>
       </c>
       <c r="D40" t="str">
-        <v>SHIVM/86365/522.65</v>
+        <v>SHIVM/86657/522.37</v>
       </c>
       <c r="E40" t="str">
-        <v>HPPL/70536/559.66</v>
+        <v>MEN/58257/625.70</v>
       </c>
       <c r="F40" t="str">
-        <v>SHPC/57473/610.55</v>
+        <v>HIDCLP/202840/213.42</v>
       </c>
     </row>
     <row r="41">
@@ -1222,19 +1222,19 @@
         <v>B49</v>
       </c>
       <c r="B41" t="str">
-        <v>SHEL/198245/284.47</v>
+        <v>SHEL/165529/286.80</v>
       </c>
       <c r="C41" t="str">
-        <v>NGPL/90209/395.85</v>
+        <v>RADHI/54582/795.67</v>
       </c>
       <c r="D41" t="str">
-        <v>RADHI/45441/793.16</v>
+        <v>SHIVM/73473/522.56</v>
       </c>
       <c r="E41" t="str">
-        <v>SHIVM/67811/522.99</v>
+        <v>NGPL/78727/396.23</v>
       </c>
       <c r="F41" t="str">
-        <v>API/94551/301.51</v>
+        <v>API/104213/301.35</v>
       </c>
     </row>
     <row r="42">
@@ -1242,19 +1242,19 @@
         <v>B50</v>
       </c>
       <c r="B42" t="str">
-        <v>RADHI/445113/796.75</v>
+        <v>RADHI/444522/797.49</v>
       </c>
       <c r="C42" t="str">
-        <v>SHEL/120721/293.55</v>
+        <v>SHEL/123722/294.84</v>
       </c>
       <c r="D42" t="str">
-        <v>NGPL/88176/388.48</v>
+        <v>SAHAS/50550/549.43</v>
       </c>
       <c r="E42" t="str">
-        <v>SAHAS/46699/549.09</v>
+        <v>SHL/45918/580.61</v>
       </c>
       <c r="F42" t="str">
-        <v>SHL/40578/580.20</v>
+        <v>NGPL/76746/389.22</v>
       </c>
     </row>
     <row r="43">
@@ -1262,19 +1262,19 @@
         <v>B51</v>
       </c>
       <c r="B43" t="str">
-        <v>AHPC/63388/299.40</v>
+        <v>AHPC/66856/299.40</v>
       </c>
       <c r="C43" t="str">
-        <v>BARUN/46099/390.71</v>
+        <v>CHDC/6422/2,608.31</v>
       </c>
       <c r="D43" t="str">
-        <v>CHDC/6422/2,608.31</v>
+        <v>BARUN/42865/390.56</v>
       </c>
       <c r="E43" t="str">
-        <v>RADHI/16021/799.76</v>
+        <v>RADHI/16050/800.39</v>
       </c>
       <c r="F43" t="str">
-        <v>AKPL/48975/265.75</v>
+        <v>AKPL/47917/266.05</v>
       </c>
     </row>
     <row r="44">
@@ -1282,19 +1282,19 @@
         <v>B52</v>
       </c>
       <c r="B44" t="str">
-        <v>HIDCLP/131012/215.96</v>
+        <v>HIDCLP/130937/215.99</v>
       </c>
       <c r="C44" t="str">
-        <v>CHDC/8471/2,602.36</v>
+        <v>CHDC/8464/2,601.77</v>
       </c>
       <c r="D44" t="str">
-        <v>SHPC/29731/608.17</v>
+        <v>SHPC/33159/611.86</v>
       </c>
       <c r="E44" t="str">
-        <v>SHIVM/25528/521.87</v>
+        <v>SHIVM/26187/521.58</v>
       </c>
       <c r="F44" t="str">
-        <v>NRN/6530/2,027.78</v>
+        <v>NRN/6378/2,026.78</v>
       </c>
     </row>
     <row r="45">
@@ -1302,19 +1302,19 @@
         <v>B53</v>
       </c>
       <c r="B45" t="str">
-        <v>MLBL/35793/391.91</v>
+        <v>MLBL/34743/391.91</v>
       </c>
       <c r="C45" t="str">
-        <v>HURJA/40322/262.91</v>
+        <v>MEN/15352/612.56</v>
       </c>
       <c r="D45" t="str">
-        <v>SHL/14397/580.61</v>
+        <v>SHL/14497/580.62</v>
       </c>
       <c r="E45" t="str">
+        <v>HURJA/31292/263.00</v>
+      </c>
+      <c r="F45" t="str">
         <v>ULBSL/2461/3,346.70</v>
-      </c>
-      <c r="F45" t="str">
-        <v>MEN/13222/611.41</v>
       </c>
     </row>
     <row r="46">
@@ -1322,16 +1322,16 @@
         <v>B54</v>
       </c>
       <c r="B46" t="str">
-        <v>UPCL/204903/466.31</v>
+        <v>UPCL/212585/465.79</v>
       </c>
       <c r="C46" t="str">
-        <v>STC/14513/5,002.83</v>
+        <v>STC/14885/5,002.90</v>
       </c>
       <c r="D46" t="str">
-        <v>CHCL/39087/562.96</v>
+        <v>CHCL/41157/563.55</v>
       </c>
       <c r="E46" t="str">
-        <v>CYCL/8431/1,668.64</v>
+        <v>CYCL/8781/1,669.06</v>
       </c>
       <c r="F46" t="str">
         <v>SADBL/24191/425.13</v>
@@ -1342,19 +1342,19 @@
         <v>B55</v>
       </c>
       <c r="B47" t="str">
-        <v>GMLI/139981/2,574.45</v>
+        <v>GMLI/150336/2,565.54</v>
       </c>
       <c r="C47" t="str">
-        <v>NRIC/261838/1,295.52</v>
+        <v>NRIC/266826/1,294.93</v>
       </c>
       <c r="D47" t="str">
-        <v>NMIC/95312/1,823.11</v>
+        <v>NMIC/99642/1,817.40</v>
       </c>
       <c r="E47" t="str">
-        <v>NLG/116118/828.81</v>
+        <v>NLG/116218/828.76</v>
       </c>
       <c r="F47" t="str">
-        <v>HRL/34451/947.00</v>
+        <v>HRL/35792/945.94</v>
       </c>
     </row>
     <row r="48">
@@ -1362,19 +1362,19 @@
         <v>B56</v>
       </c>
       <c r="B48" t="str">
-        <v>UPCL/199657/458.01</v>
+        <v>BPCL/148070/726.91</v>
       </c>
       <c r="C48" t="str">
-        <v>NGPL/215567/402.22</v>
+        <v>UPCL/186491/457.63</v>
       </c>
       <c r="D48" t="str">
-        <v>BPCL/97959/705.61</v>
+        <v>NGPL/179552/402.45</v>
       </c>
       <c r="E48" t="str">
-        <v>SMHL/46611/1,002.07</v>
+        <v>SMHL/50411/1,003.33</v>
       </c>
       <c r="F48" t="str">
-        <v>BEDC/47456/706.74</v>
+        <v>HIDCLP/137564/218.86</v>
       </c>
     </row>
     <row r="49">
@@ -1382,19 +1382,19 @@
         <v>B57</v>
       </c>
       <c r="B49" t="str">
-        <v>CHCL/71810/565.56</v>
+        <v>CHCL/77600/566.26</v>
       </c>
       <c r="C49" t="str">
-        <v>MEN/54540/607.02</v>
+        <v>UPCL/62928/452.30</v>
       </c>
       <c r="D49" t="str">
-        <v>UPCL/67631/452.21</v>
+        <v>MEN/46712/607.75</v>
       </c>
       <c r="E49" t="str">
-        <v>AHPC/93456/297.85</v>
+        <v>NTC/31762/853.65</v>
       </c>
       <c r="F49" t="str">
-        <v>RFPL/44708/561.33</v>
+        <v>AKPL/86291/275.15</v>
       </c>
     </row>
     <row r="50">
@@ -1402,19 +1402,19 @@
         <v>B58</v>
       </c>
       <c r="B50" t="str">
-        <v>KBL/1204937/214.15</v>
+        <v>KBL/1208893/214.13</v>
       </c>
       <c r="C50" t="str">
-        <v>NRN/95569/2,031.64</v>
+        <v>HPPL/330683/537.73</v>
       </c>
       <c r="D50" t="str">
-        <v>HPPL/329422/536.57</v>
+        <v>NRN/88808/2,031.57</v>
       </c>
       <c r="E50" t="str">
-        <v>HIDCLP/762569/218.74</v>
+        <v>HIDCLP/811778/218.79</v>
       </c>
       <c r="F50" t="str">
-        <v>LSL/467112/220.43</v>
+        <v>LSL/467286/220.42</v>
       </c>
     </row>
     <row r="51">
@@ -1422,19 +1422,19 @@
         <v>B59</v>
       </c>
       <c r="B51" t="str">
-        <v>API/172476/302.12</v>
+        <v>API/170758/302.05</v>
       </c>
       <c r="C51" t="str">
-        <v>SHIVM/52592/522.46</v>
+        <v>SHIVM/54462/522.27</v>
       </c>
       <c r="D51" t="str">
-        <v>AHPC/51653/301.36</v>
+        <v>AHPC/57613/301.19</v>
       </c>
       <c r="E51" t="str">
         <v>ALICL/23460/680.44</v>
       </c>
       <c r="F51" t="str">
-        <v>HIDCLP/69196/213.82</v>
+        <v>HIDCLP/68118/213.87</v>
       </c>
     </row>
     <row r="52">
@@ -1442,19 +1442,19 @@
         <v>B60</v>
       </c>
       <c r="B52" t="str">
-        <v>RADHI/120132/802.29</v>
+        <v>SHPC/137760/631.84</v>
       </c>
       <c r="C52" t="str">
-        <v>SHPC/131142/630.29</v>
+        <v>RADHI/102477/802.65</v>
       </c>
       <c r="D52" t="str">
-        <v>BPCL/76203/703.95</v>
+        <v>BPCL/76018/704.30</v>
       </c>
       <c r="E52" t="str">
-        <v>SHL/92081/577.61</v>
+        <v>SHL/92381/577.68</v>
       </c>
       <c r="F52" t="str">
-        <v>HPPL/89181/529.41</v>
+        <v>UMHL/79015/539.56</v>
       </c>
     </row>
     <row r="53">
@@ -1462,19 +1462,19 @@
         <v>B61</v>
       </c>
       <c r="B53" t="str">
-        <v>RADHI/51178/815.09</v>
+        <v>RADHI/108296/823.31</v>
       </c>
       <c r="C53" t="str">
-        <v>NGPL/51970/400.65</v>
+        <v>CHDC/8109/2,617.28</v>
       </c>
       <c r="D53" t="str">
-        <v>CHDC/8109/2,617.28</v>
+        <v>UNHPL/40584/410.53</v>
       </c>
       <c r="E53" t="str">
-        <v>HIDCL/54149/308.72</v>
+        <v>NGPL/39740/400.65</v>
       </c>
       <c r="F53" t="str">
-        <v>HIDCLP/51753/218.27</v>
+        <v>HIDCL/46049/308.72</v>
       </c>
     </row>
     <row r="54">
@@ -1482,19 +1482,19 @@
         <v>B62</v>
       </c>
       <c r="B54" t="str">
-        <v>UMHL/271161/515.87</v>
+        <v>UNHPL/257137/388.89</v>
       </c>
       <c r="C54" t="str">
-        <v>UNHPL/252275/383.93</v>
+        <v>RADHI/76585/800.25</v>
       </c>
       <c r="D54" t="str">
-        <v>RADHI/77793/800.14</v>
+        <v>SPDL/91293/419.59</v>
       </c>
       <c r="E54" t="str">
-        <v>SPDL/99832/417.90</v>
+        <v>UMHL/78071/516.12</v>
       </c>
       <c r="F54" t="str">
-        <v>ANLB/4513/5,394.85</v>
+        <v>ANLB/4356/5,394.85</v>
       </c>
     </row>
     <row r="55">
@@ -1502,19 +1502,19 @@
         <v>B63</v>
       </c>
       <c r="B55" t="str">
-        <v>RADHI/49873/798.95</v>
+        <v>RADHI/51890/801.82</v>
       </c>
       <c r="C55" t="str">
-        <v>OMPL/9607/1,716.26</v>
+        <v>OMPL/8897/1,705.42</v>
       </c>
       <c r="D55" t="str">
         <v>NBL/55325/256.36</v>
       </c>
       <c r="E55" t="str">
-        <v>PPCL/41217/335.15</v>
+        <v>PPCL/33967/335.15</v>
       </c>
       <c r="F55" t="str">
-        <v>CHCL/22047/554.51</v>
+        <v>SHL/15408/581.78</v>
       </c>
     </row>
     <row r="56">
@@ -1522,19 +1522,19 @@
         <v>B64</v>
       </c>
       <c r="B56" t="str">
-        <v>BPCL/397155/646.94</v>
+        <v>BPCL/382176/651.47</v>
       </c>
       <c r="C56" t="str">
-        <v>NRN/19149/2,062.74</v>
+        <v>UNHPL/116881/415.81</v>
       </c>
       <c r="D56" t="str">
-        <v>UNHPL/81355/399.69</v>
+        <v>NRN/17984/2,062.74</v>
       </c>
       <c r="E56" t="str">
-        <v>SHL/52487/582.81</v>
+        <v>SHL/53287/582.84</v>
       </c>
       <c r="F56" t="str">
-        <v>CHDC/8881/2,564.01</v>
+        <v>MERO/36828/738.72</v>
       </c>
     </row>
     <row r="57">
@@ -1542,16 +1542,16 @@
         <v>B65</v>
       </c>
       <c r="B57" t="str">
-        <v>SARBTM/55580/841.40</v>
+        <v>SARBTM/55384/841.44</v>
       </c>
       <c r="C57" t="str">
-        <v>RFPL/70401/623.09</v>
+        <v>RFPL/64422/622.80</v>
       </c>
       <c r="D57" t="str">
-        <v>NIFRA/130337/282.68</v>
+        <v>SHPC/63304/612.39</v>
       </c>
       <c r="E57" t="str">
-        <v>SHPC/57827/609.56</v>
+        <v>NIFRA/132539/282.65</v>
       </c>
       <c r="F57" t="str">
         <v>SANIMA/106987/318.67</v>
@@ -1565,16 +1565,16 @@
         <v>HIDCL/96377/304.77</v>
       </c>
       <c r="C58" t="str">
-        <v>CHDC/8542/2,588.35</v>
+        <v>CHDC/9077/2,586.56</v>
       </c>
       <c r="D58" t="str">
-        <v>BPCL/29344/654.68</v>
+        <v>BPCL/34824/678.16</v>
       </c>
       <c r="E58" t="str">
-        <v>NRN/6093/2,026.41</v>
+        <v>NRN/7437/2,024.15</v>
       </c>
       <c r="F58" t="str">
-        <v>NGPL/29841/383.59</v>
+        <v>SBL/30841/301.24</v>
       </c>
     </row>
     <row r="59">
@@ -1582,19 +1582,19 @@
         <v>B67</v>
       </c>
       <c r="B59" t="str">
-        <v>RADHI/153398/786.20</v>
+        <v>RADHI/152648/786.27</v>
       </c>
       <c r="C59" t="str">
-        <v>HIDCL/168256/303.93</v>
+        <v>HIDCL/169206/303.90</v>
       </c>
       <c r="D59" t="str">
-        <v>MEN/45626/621.38</v>
+        <v>NGPL/90022/397.68</v>
       </c>
       <c r="E59" t="str">
-        <v>NGPL/65659/396.45</v>
+        <v>MEN/46066/621.54</v>
       </c>
       <c r="F59" t="str">
-        <v>UMHL/47870/511.55</v>
+        <v>UMHL/43337/511.92</v>
       </c>
     </row>
     <row r="60">
@@ -1602,19 +1602,19 @@
         <v>B68</v>
       </c>
       <c r="B60" t="str">
-        <v>HIDCLP/230535/211.74</v>
+        <v>HIDCLP/240105/211.96</v>
       </c>
       <c r="C60" t="str">
-        <v>NGPL/85159/387.64</v>
+        <v>NGPL/65988/388.00</v>
       </c>
       <c r="D60" t="str">
-        <v>BPCL/29230/596.91</v>
+        <v>BPCL/30221/602.31</v>
       </c>
       <c r="E60" t="str">
-        <v>AHPC/54836/299.27</v>
+        <v>UPCL/40961/447.69</v>
       </c>
       <c r="F60" t="str">
-        <v>UPCL/34135/447.34</v>
+        <v>AHPC/60275/299.27</v>
       </c>
     </row>
     <row r="61">
@@ -1622,19 +1622,19 @@
         <v>B69</v>
       </c>
       <c r="B61" t="str">
-        <v>BPCL/108169/713.11</v>
+        <v>BPCL/131480/734.34</v>
       </c>
       <c r="C61" t="str">
-        <v>SHL/99531/579.00</v>
+        <v>SHL/101534/579.29</v>
       </c>
       <c r="D61" t="str">
-        <v>SPDL/53053/427.77</v>
+        <v>SPDL/73753/433.03</v>
       </c>
       <c r="E61" t="str">
-        <v>SHEL/62622/289.99</v>
+        <v>CHDC/4400/2,573.09</v>
       </c>
       <c r="F61" t="str">
-        <v>CHDC/4340/2,573.38</v>
+        <v>EBL/14550/646.92</v>
       </c>
     </row>
     <row r="62">
@@ -1642,19 +1642,19 @@
         <v>B70</v>
       </c>
       <c r="B62" t="str">
-        <v>UNHPL/81017/391.31</v>
+        <v>BPCL/68571/644.92</v>
       </c>
       <c r="C62" t="str">
-        <v>BPCL/54551/626.95</v>
+        <v>UNHPL/76145/399.94</v>
       </c>
       <c r="D62" t="str">
-        <v>UPCL/35817/451.07</v>
+        <v>UPCL/36047/451.10</v>
       </c>
       <c r="E62" t="str">
-        <v>PRVU/71940/217.43</v>
+        <v>PRVU/70540/217.43</v>
       </c>
       <c r="F62" t="str">
-        <v>RADHI/16228/793.95</v>
+        <v>HIDCLP/66070/215.60</v>
       </c>
     </row>
     <row r="63">
@@ -1662,19 +1662,19 @@
         <v>B71</v>
       </c>
       <c r="B63" t="str">
-        <v>SHPC/32551/642.96</v>
+        <v>CHDC/9994/2,600.28</v>
       </c>
       <c r="C63" t="str">
-        <v>CHDC/8839/2,603.75</v>
+        <v>SHPC/32421/643.85</v>
       </c>
       <c r="D63" t="str">
-        <v>RADHI/19455/793.01</v>
+        <v>RADHI/28345/794.93</v>
       </c>
       <c r="E63" t="str">
-        <v>UPCL/33408/446.71</v>
+        <v>UPCL/31278/446.73</v>
       </c>
       <c r="F63" t="str">
-        <v>HIDCL/37141/311.05</v>
+        <v>HIDCL/41241/310.70</v>
       </c>
     </row>
     <row r="64">
@@ -1682,19 +1682,19 @@
         <v>B72</v>
       </c>
       <c r="B64" t="str">
-        <v>CORBL/37887/2,394.99</v>
+        <v>JOSHI/196157/432.34</v>
       </c>
       <c r="C64" t="str">
-        <v>SAPDBL/30099/992.80</v>
+        <v>CORBL/31240/2,395.03</v>
       </c>
       <c r="D64" t="str">
-        <v>NRN/7566/2,037.62</v>
+        <v>NRN/7716/2,037.25</v>
       </c>
       <c r="E64" t="str">
         <v>KBL/60299/208.32</v>
       </c>
       <c r="F64" t="str">
-        <v>LBBL/27251/447.53</v>
+        <v>LBBL/26251/447.53</v>
       </c>
     </row>
     <row r="65">
@@ -1702,19 +1702,19 @@
         <v>B73</v>
       </c>
       <c r="B65" t="str">
-        <v>TVCL/780/472.13</v>
+        <v>NICA/1000/343.00</v>
       </c>
       <c r="C65" t="str">
-        <v>NICA/1000/343.00</v>
+        <v>BHL/1400/211.96</v>
       </c>
       <c r="D65" t="str">
-        <v>BHL/1400/211.96</v>
+        <v>RHGCL/480/554.96</v>
       </c>
       <c r="E65" t="str">
-        <v>RHGCL/480/554.96</v>
+        <v>CHDC/82/2,712.71</v>
       </c>
       <c r="F65" t="str">
-        <v>CHDC/82/2,712.71</v>
+        <v>SONA/300/453.00</v>
       </c>
     </row>
     <row r="66">
@@ -1722,19 +1722,19 @@
         <v>B74</v>
       </c>
       <c r="B66" t="str">
-        <v>RADHI/68810/826.55</v>
+        <v>RADHI/68810/826.67</v>
       </c>
       <c r="C66" t="str">
-        <v>SAPDBL/29371/1,036.04</v>
+        <v>SAPDBL/29960/1,031.19</v>
       </c>
       <c r="D66" t="str">
-        <v>SKBBL/17007/802.67</v>
+        <v>SKBBL/18291/801.83</v>
       </c>
       <c r="E66" t="str">
         <v>NABIL/22068/493.34</v>
       </c>
       <c r="F66" t="str">
-        <v>NLIC/12962/755.06</v>
+        <v>NLIC/13586/754.48</v>
       </c>
     </row>
     <row r="67">
@@ -1742,19 +1742,19 @@
         <v>B75</v>
       </c>
       <c r="B67" t="str">
-        <v>CGH/33642/996.44</v>
+        <v>BPCL/46352/707.00</v>
       </c>
       <c r="C67" t="str">
-        <v>BPCL/40577/698.27</v>
+        <v>CGH/32547/997.32</v>
       </c>
       <c r="D67" t="str">
-        <v>SHPC/27091/632.64</v>
+        <v>HIDCLP/59256/222.14</v>
       </c>
       <c r="E67" t="str">
-        <v>HIDCLP/62256/222.16</v>
+        <v>SHPC/14924/633.48</v>
       </c>
       <c r="F67" t="str">
-        <v>RADHI/17396/780.03</v>
+        <v>HDHPC/43525/202.89</v>
       </c>
     </row>
     <row r="68">
@@ -1762,19 +1762,19 @@
         <v>B76</v>
       </c>
       <c r="B68" t="str">
-        <v>BPCL/81431/733.61</v>
+        <v>BPCL/80503/733.76</v>
       </c>
       <c r="C68" t="str">
-        <v>SHIVM/22677/519.75</v>
+        <v>SHIVM/23177/519.64</v>
       </c>
       <c r="D68" t="str">
-        <v>UMRH/6634/623.68</v>
+        <v>UMRH/6654/623.61</v>
       </c>
       <c r="E68" t="str">
-        <v>HIDCL/9526/314.20</v>
+        <v>HIDCL/9156/314.00</v>
       </c>
       <c r="F68" t="str">
-        <v>MEN/4614/581.73</v>
+        <v>AHPC/8251/300.58</v>
       </c>
     </row>
     <row r="69">
@@ -1782,19 +1782,19 @@
         <v>B77</v>
       </c>
       <c r="B69" t="str">
-        <v>BPCL/313024/632.03</v>
+        <v>BPCL/326188/640.47</v>
       </c>
       <c r="C69" t="str">
-        <v>NGPL/144259/403.11</v>
+        <v>NGPL/316069/405.98</v>
       </c>
       <c r="D69" t="str">
-        <v>AHPC/118148/306.45</v>
+        <v>HIDCLP/182615/216.58</v>
       </c>
       <c r="E69" t="str">
-        <v>HIDCLP/125990/215.67</v>
+        <v>AHPC/106418/306.44</v>
       </c>
       <c r="F69" t="str">
-        <v>MEN/39148/615.02</v>
+        <v>MEN/39288/615.03</v>
       </c>
     </row>
     <row r="70">
@@ -1802,19 +1802,19 @@
         <v>B78</v>
       </c>
       <c r="B70" t="str">
-        <v>CHDC/2956/2,643.70</v>
+        <v>CHDC/2981/2,643.09</v>
       </c>
       <c r="C70" t="str">
-        <v>ALICL/7268/690.33</v>
+        <v>ALICL/7249/690.33</v>
       </c>
       <c r="D70" t="str">
         <v>HIDCLP/21213/219.29</v>
       </c>
       <c r="E70" t="str">
-        <v>NGPL/10199/396.41</v>
+        <v>NGPL/10182/396.41</v>
       </c>
       <c r="F70" t="str">
-        <v>SINDU/3520/846.36</v>
+        <v>SINDU/4170/832.51</v>
       </c>
     </row>
     <row r="71">
@@ -1842,19 +1842,19 @@
         <v>B80</v>
       </c>
       <c r="B72" t="str">
-        <v>NIFRA/92287/287.08</v>
+        <v>NIFRA/91687/287.08</v>
       </c>
       <c r="C72" t="str">
-        <v>NMLBBL/38733/658.87</v>
+        <v>NMLBBL/38753/658.57</v>
       </c>
       <c r="D72" t="str">
-        <v>CHCL/23811/551.77</v>
+        <v>CHCL/24161/552.05</v>
       </c>
       <c r="E72" t="str">
-        <v>USLB/7033/1,849.46</v>
+        <v>USLB/6816/1,849.46</v>
       </c>
       <c r="F72" t="str">
-        <v>MEN/22955/590.92</v>
+        <v>MEN/21855/590.92</v>
       </c>
     </row>
     <row r="73">
@@ -1862,19 +1862,19 @@
         <v>B81</v>
       </c>
       <c r="B73" t="str">
-        <v>CHCL/133105/563.24</v>
+        <v>CHCL/145205/564.27</v>
       </c>
       <c r="C73" t="str">
-        <v>NGPL/161775/396.21</v>
+        <v>NGPL/153355/396.43</v>
       </c>
       <c r="D73" t="str">
-        <v>HRL/44828/965.59</v>
+        <v>HRL/47538/963.27</v>
       </c>
       <c r="E73" t="str">
-        <v>SHPC/54976/607.90</v>
+        <v>SHPC/64691/609.93</v>
       </c>
       <c r="F73" t="str">
-        <v>CHDC/9296/2,614.60</v>
+        <v>SHEL/85446/303.66</v>
       </c>
     </row>
     <row r="74">
@@ -1882,19 +1882,19 @@
         <v>B82</v>
       </c>
       <c r="B74" t="str">
-        <v>SHPC/49633/602.40</v>
+        <v>NRN/10135/2,043.73</v>
       </c>
       <c r="C74" t="str">
-        <v>NRN/10085/2,043.78</v>
+        <v>SHPC/41156/603.29</v>
       </c>
       <c r="D74" t="str">
-        <v>BPCL/15024/664.96</v>
+        <v>BPCL/15009/670.39</v>
       </c>
       <c r="E74" t="str">
-        <v>NGPL/25165/407.99</v>
+        <v>NICA/25422/372.12</v>
       </c>
       <c r="F74" t="str">
-        <v>NICA/25422/372.12</v>
+        <v>HRL/10704/951.92</v>
       </c>
     </row>
     <row r="75">
@@ -1902,13 +1902,13 @@
         <v>B83</v>
       </c>
       <c r="B75" t="str">
-        <v>HRL/29387/942.39</v>
+        <v>HRL/31387/940.79</v>
       </c>
       <c r="C75" t="str">
-        <v>NGPL/54985/401.66</v>
+        <v>NGPL/56107/401.79</v>
       </c>
       <c r="D75" t="str">
-        <v>SHPC/25918/627.47</v>
+        <v>SHPC/23268/628.41</v>
       </c>
       <c r="E75" t="str">
         <v>KPCL/20408/520.95</v>
@@ -1922,19 +1922,19 @@
         <v>B84</v>
       </c>
       <c r="B76" t="str">
-        <v>BPCL/54547/727.70</v>
+        <v>BPCL/60347/736.82</v>
       </c>
       <c r="C76" t="str">
-        <v>UPCL/84340/451.58</v>
+        <v>UPCL/86210/451.57</v>
       </c>
       <c r="D76" t="str">
+        <v>SADBL/75447/419.42</v>
+      </c>
+      <c r="E76" t="str">
         <v>HIDCL/98916/308.15</v>
       </c>
-      <c r="E76" t="str">
-        <v>SADBL/67875/421.04</v>
-      </c>
       <c r="F76" t="str">
-        <v>NGPL/63410/400.76</v>
+        <v>MKHL/36964/742.33</v>
       </c>
     </row>
     <row r="77">
@@ -1942,16 +1942,16 @@
         <v>B85</v>
       </c>
       <c r="B77" t="str">
-        <v>NGPL/233345/385.39</v>
+        <v>NGPL/245457/386.08</v>
       </c>
       <c r="C77" t="str">
-        <v>AHPC/86354/298.34</v>
+        <v>AHPC/87654/298.35</v>
       </c>
       <c r="D77" t="str">
-        <v>API/68186/302.76</v>
+        <v>API/69066/302.71</v>
       </c>
       <c r="E77" t="str">
-        <v>SHL/34921/584.18</v>
+        <v>SHL/35521/584.18</v>
       </c>
       <c r="F77" t="str">
         <v>SAHAS/27375/539.22</v>
@@ -1962,19 +1962,19 @@
         <v>B86</v>
       </c>
       <c r="B78" t="str">
-        <v>RADHI/31645/802.16</v>
+        <v>RADHI/32445/803.40</v>
       </c>
       <c r="C78" t="str">
-        <v>SHPC/26093/620.85</v>
+        <v>SHPC/34398/625.12</v>
       </c>
       <c r="D78" t="str">
-        <v>AKPL/30129/273.10</v>
+        <v>AKPL/30129/273.17</v>
       </c>
       <c r="E78" t="str">
+        <v>HURJA/28544/264.00</v>
+      </c>
+      <c r="F78" t="str">
         <v>NRN/3764/2,023.67</v>
-      </c>
-      <c r="F78" t="str">
-        <v>API/24520/299.69</v>
       </c>
     </row>
     <row r="79">
@@ -1982,19 +1982,19 @@
         <v>B87</v>
       </c>
       <c r="B79" t="str">
-        <v>RADHI/46393/805.12</v>
+        <v>BPCL/45815/744.11</v>
       </c>
       <c r="C79" t="str">
-        <v>BPCL/45810/741.74</v>
+        <v>RADHI/43283/807.47</v>
       </c>
       <c r="D79" t="str">
-        <v>CGH/8375/983.56</v>
+        <v>CGH/8369/986.37</v>
       </c>
       <c r="E79" t="str">
-        <v>NGPL/20266/389.48</v>
+        <v>GCIL/15198/511.72</v>
       </c>
       <c r="F79" t="str">
-        <v>AKPL/19202/281.15</v>
+        <v>NGPL/18616/389.48</v>
       </c>
     </row>
     <row r="80">
@@ -2002,19 +2002,19 @@
         <v>B88</v>
       </c>
       <c r="B80" t="str">
-        <v>SAPDBL/57028/1,049.78</v>
+        <v>SAPDBL/56511/1,049.69</v>
       </c>
       <c r="C80" t="str">
-        <v>CHCL/52076/568.72</v>
+        <v>CHCL/46179/568.75</v>
       </c>
       <c r="D80" t="str">
-        <v>CHDC/6080/2,583.07</v>
+        <v>NHPC/62613/222.68</v>
       </c>
       <c r="E80" t="str">
         <v>CORBL/4693/2,617.66</v>
       </c>
       <c r="F80" t="str">
-        <v>NHPC/51141/223.10</v>
+        <v>CHDC/4430/2,583.00</v>
       </c>
     </row>
     <row r="81">
@@ -2025,16 +2025,16 @@
         <v>GBIME/115853/238.63</v>
       </c>
       <c r="C81" t="str">
-        <v>BPCL/14320/690.01</v>
+        <v>CGH/10706/976.72</v>
       </c>
       <c r="D81" t="str">
-        <v>CGH/8106/967.10</v>
+        <v>BPCL/14010/692.82</v>
       </c>
       <c r="E81" t="str">
-        <v>UNHPL/17221/412.54</v>
+        <v>UNHPL/22951/421.63</v>
       </c>
       <c r="F81" t="str">
-        <v>MEN/8613/616.04</v>
+        <v>MEN/9613/616.76</v>
       </c>
     </row>
     <row r="82">
@@ -2042,13 +2042,13 @@
         <v>B90</v>
       </c>
       <c r="B82" t="str">
-        <v>HBL/113477/229.38</v>
+        <v>HBL/114477/229.17</v>
       </c>
       <c r="C82" t="str">
-        <v>API/58279/311.26</v>
+        <v>API/59629/310.93</v>
       </c>
       <c r="D82" t="str">
-        <v>SHPC/13752/627.50</v>
+        <v>SHPC/13252/627.54</v>
       </c>
       <c r="E82" t="str">
         <v>EBL/11126/631.20</v>
@@ -2062,19 +2062,19 @@
         <v>B91</v>
       </c>
       <c r="B83" t="str">
-        <v>RADHI/26644/796.99</v>
+        <v>RADHI/44363/802.12</v>
       </c>
       <c r="C83" t="str">
-        <v>NGPL/51677/393.40</v>
+        <v>BPCL/40118/698.85</v>
       </c>
       <c r="D83" t="str">
-        <v>BPCL/29649/670.68</v>
+        <v>CGH/16083/980.79</v>
       </c>
       <c r="E83" t="str">
-        <v>SARBTM/17594/843.02</v>
+        <v>SARBTM/17045/843.02</v>
       </c>
       <c r="F83" t="str">
-        <v>CHDC/5395/2,613.34</v>
+        <v>CHDC/5285/2,611.57</v>
       </c>
     </row>
     <row r="84">
@@ -2082,19 +2082,19 @@
         <v>B92</v>
       </c>
       <c r="B84" t="str">
-        <v>HIDCL/108971/303.82</v>
+        <v>HIDCL/119531/303.77</v>
       </c>
       <c r="C84" t="str">
-        <v>UPCL/36157/451.01</v>
+        <v>UPCL/39957/451.05</v>
       </c>
       <c r="D84" t="str">
-        <v>SHPC/18210/622.38</v>
+        <v>SHPC/16990/626.14</v>
       </c>
       <c r="E84" t="str">
-        <v>NGPL/19838/391.45</v>
+        <v>BPCL/10075/698.80</v>
       </c>
       <c r="F84" t="str">
-        <v>HRL/7729/956.16</v>
+        <v>NGPL/19028/391.61</v>
       </c>
     </row>
     <row r="85">
@@ -2102,7 +2102,7 @@
         <v>B93</v>
       </c>
       <c r="B85" t="str">
-        <v>MBJC/21250/335.67</v>
+        <v>MBJC/30661/334.45</v>
       </c>
       <c r="C85" t="str">
         <v>AKPL/22400/288.71</v>
@@ -2114,7 +2114,7 @@
         <v>MPFL/4420/614.53</v>
       </c>
       <c r="F85" t="str">
-        <v>CHCL/3727/547.24</v>
+        <v>CHCL/3800/547.64</v>
       </c>
     </row>
     <row r="86">
@@ -2122,19 +2122,19 @@
         <v>B94</v>
       </c>
       <c r="B86" t="str">
-        <v>RADHI/121500/792.89</v>
+        <v>RADHI/115661/793.48</v>
       </c>
       <c r="C86" t="str">
-        <v>MKHL/29722/745.21</v>
+        <v>MKHL/30282/745.20</v>
       </c>
       <c r="D86" t="str">
-        <v>NGPL/59209/393.50</v>
+        <v>SHL/32900/571.60</v>
       </c>
       <c r="E86" t="str">
-        <v>SHL/31700/571.31</v>
+        <v>PRIN/17725/844.95</v>
       </c>
       <c r="F86" t="str">
-        <v>PRIN/17725/844.95</v>
+        <v>SHIVM/26928/519.04</v>
       </c>
     </row>
     <row r="87">
@@ -2142,16 +2142,16 @@
         <v>B95</v>
       </c>
       <c r="B87" t="str">
-        <v>NGPL/71327/398.62</v>
+        <v>NGPL/65337/398.69</v>
       </c>
       <c r="C87" t="str">
-        <v>SHPC/37097/608.07</v>
+        <v>RADHI/22762/820.38</v>
       </c>
       <c r="D87" t="str">
-        <v>RADHI/21874/819.84</v>
+        <v>SHPC/29047/609.82</v>
       </c>
       <c r="E87" t="str">
-        <v>UPCL/31271/454.84</v>
+        <v>UPCL/28698/454.86</v>
       </c>
       <c r="F87" t="str">
         <v>NRN/4863/2,058.99</v>
@@ -2162,19 +2162,19 @@
         <v>B96</v>
       </c>
       <c r="B88" t="str">
-        <v>NRN/34584/2,043.38</v>
+        <v>NRN/33552/2,043.38</v>
       </c>
       <c r="C88" t="str">
-        <v>BPCL/56219/705.00</v>
+        <v>BPCL/66880/722.70</v>
       </c>
       <c r="D88" t="str">
-        <v>NICA/104431/365.65</v>
+        <v>NICA/104506/365.63</v>
       </c>
       <c r="E88" t="str">
-        <v>RADHI/38032/824.08</v>
+        <v>RADHI/36032/824.08</v>
       </c>
       <c r="F88" t="str">
-        <v>SHPC/50186/620.98</v>
+        <v>SHPC/30789/620.98</v>
       </c>
     </row>
     <row r="89">
@@ -2182,19 +2182,19 @@
         <v>B97</v>
       </c>
       <c r="B89" t="str">
-        <v>SADBL/23762/418.13</v>
+        <v>SHEL/46390/305.20</v>
       </c>
       <c r="C89" t="str">
-        <v>NRN/4572/2,027.62</v>
+        <v>NRN/4522/2,027.24</v>
       </c>
       <c r="D89" t="str">
-        <v>UPCL/19199/451.58</v>
+        <v>UPCL/19617/451.60</v>
       </c>
       <c r="E89" t="str">
-        <v>MEN/12450/632.82</v>
+        <v>MEN/13150/631.34</v>
       </c>
       <c r="F89" t="str">
-        <v>SPDL/13796/401.84</v>
+        <v>SADBL/16362/418.13</v>
       </c>
     </row>
     <row r="90">
@@ -2202,19 +2202,19 @@
         <v>B98</v>
       </c>
       <c r="B90" t="str">
-        <v>BPCL/54540/755.66</v>
+        <v>BPCL/46850/755.66</v>
       </c>
       <c r="C90" t="str">
-        <v>OMPL/9270/1,809.07</v>
+        <v>OMPL/9470/1,800.72</v>
       </c>
       <c r="D90" t="str">
         <v>AKPL/50024/283.71</v>
       </c>
       <c r="E90" t="str">
-        <v>SCB/11873/611.81</v>
+        <v>UNHPL/26525/418.57</v>
       </c>
       <c r="F90" t="str">
-        <v>SHIVM/12210/523.97</v>
+        <v>SCB/12167/611.86</v>
       </c>
     </row>
     <row r="91">
@@ -2222,19 +2222,19 @@
         <v>B99</v>
       </c>
       <c r="B91" t="str">
-        <v>SHEL/53965/296.49</v>
+        <v>SHEL/66715/301.06</v>
       </c>
       <c r="C91" t="str">
-        <v>BPCL/15186/653.78</v>
+        <v>HIDCLP/59115/212.58</v>
       </c>
       <c r="D91" t="str">
-        <v>CGH/8086/994.57</v>
+        <v>CGH/6086/994.57</v>
       </c>
       <c r="E91" t="str">
-        <v>CHDC/2190/2,618.80</v>
+        <v>CHDC/2140/2,618.80</v>
       </c>
       <c r="F91" t="str">
-        <v>HIDCLP/30115/210.30</v>
+        <v>RHPL/13287/418.55</v>
       </c>
     </row>
     <row r="92">
@@ -2242,16 +2242,16 @@
         <v>B100</v>
       </c>
       <c r="B92" t="str">
-        <v>MLBL/159943/389.05</v>
+        <v>MLBL/169941/388.92</v>
       </c>
       <c r="C92" t="str">
-        <v>KSBBL/57693/449.75</v>
+        <v>KSBBL/62692/449.50</v>
       </c>
       <c r="D92" t="str">
-        <v>PHCL/44005/581.11</v>
+        <v>PHCL/44045/581.04</v>
       </c>
       <c r="E92" t="str">
-        <v>BPCL/28853/739.80</v>
+        <v>BPCL/30407/760.95</v>
       </c>
       <c r="F92" t="str">
         <v>LBBL/44169/448.48</v>
@@ -2265,16 +2265,16 @@
         <v>AHPC/37574/305.90</v>
       </c>
       <c r="C93" t="str">
-        <v>CHDC/4087/2,645.00</v>
+        <v>HIDCLP/52850/218.54</v>
       </c>
       <c r="D93" t="str">
-        <v>HIDCLP/48250/217.46</v>
+        <v>AKPL/35200/276.61</v>
       </c>
       <c r="E93" t="str">
-        <v>AKPL/35550/276.61</v>
+        <v>CHDC/2587/2,645.00</v>
       </c>
       <c r="F93" t="str">
-        <v>RADHI/9917/817.89</v>
+        <v>RADHI/8467/817.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>